<commit_message>
remove remaining emmo-related files and modules, minor repository restructuration
</commit_message>
<xml_diff>
--- a/tests/csv_pipeline_test/output/DX56_D_FZ2_WR00_43.generic.xlsx
+++ b/tests/csv_pipeline_test/output/DX56_D_FZ2_WR00_43.generic.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://www.test2.de</t>
+          <t>https://www.example.org/</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>86491bcc-2465-45f8-a025-afe4dc59f7c9</t>
+          <t>4430481c-38f0-4d6f-a107-f7de0d4a95a0</t>
         </is>
       </c>
     </row>

</xml_diff>